<commit_message>
Ajout de spécifications dans les scénarios
</commit_message>
<xml_diff>
--- a/Documentation/UseCases - Scenarios/Scenarios/ScenariosAdmin.xlsx
+++ b/Documentation/UseCases - Scenarios/Scenarios/ScenariosAdmin.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Axel.PITTET\Documents\GitHub\TPI_2023\Rapport de projet\UseCases - Scenarios\Scenarios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Axel.PITTET\Documents\GitHub\TPI_2023\Documentation\UseCases - Scenarios\Scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57AC2783-8977-447A-B70A-AB6FEBB28334}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBC33122-6AA9-4C9F-BF71-7EB021976C1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="2430" windowWidth="21600" windowHeight="11835" xr2:uid="{3CC9808D-9F48-48C1-8654-DA68AC4A64CA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{3CC9808D-9F48-48C1-8654-DA68AC4A64CA}"/>
   </bookViews>
   <sheets>
     <sheet name="CRUD Locations" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="25">
   <si>
     <t>Action utilisateur</t>
   </si>
@@ -44,9 +44,6 @@
   </si>
   <si>
     <t>Réaction</t>
-  </si>
-  <si>
-    <t>Tout les champs sont remplis</t>
   </si>
   <si>
     <t>Affiche la page de gestion administrateur</t>
@@ -596,8 +593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35E9A2F3-5107-4346-894D-895830D3B2A8}">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -607,7 +604,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -625,20 +622,20 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -653,45 +650,45 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -706,45 +703,45 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -759,45 +756,45 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -830,8 +827,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67C2BFF1-D369-412D-9557-51B2637A757B}">
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -841,7 +838,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -859,20 +856,20 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -887,45 +884,45 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -940,45 +937,45 @@
     </row>
     <row r="14" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -993,45 +990,45 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>